<commit_message>
edit all java projects - now we create arrays per list and not an array of arrays on every list
</commit_message>
<xml_diff>
--- a/Benchmarks/benchmarkPlan.xlsx
+++ b/Benchmarks/benchmarkPlan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yyakobi\Documents\GitHub\LeapList\Benchmarks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="22980" windowHeight="9555"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Benchmarks</t>
   </si>
@@ -81,39 +86,18 @@
     <t>What happens when all nodes compete on the same area</t>
   </si>
   <si>
-    <t>ins</t>
-  </si>
-  <si>
-    <t>rem</t>
-  </si>
-  <si>
-    <t>rq</t>
-  </si>
-  <si>
-    <t>look</t>
-  </si>
-  <si>
-    <t>Benchmark pecentage of run time per method? When equally distrbuted?</t>
-  </si>
-  <si>
-    <t>Also check HW for other benchmarks ideas</t>
-  </si>
-  <si>
-    <t>Who gets to 10000000 Elements</t>
-  </si>
-  <si>
-    <t>One thread executing logic only! Overhead of code complexity</t>
+    <t>yossi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -193,12 +177,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -240,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -272,9 +259,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -306,6 +294,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -481,18 +470,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -531,7 +520,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="42.75">
+    <row r="3" spans="1:10" ht="45">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -551,7 +540,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="57">
+    <row r="4" spans="1:10" ht="60">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -564,14 +553,16 @@
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="28.5">
+    <row r="5" spans="1:10" ht="30">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -589,7 +580,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="28.5">
+    <row r="6" spans="1:10" ht="30">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -609,7 +600,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="28.5">
+    <row r="7" spans="1:10" ht="45">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -620,14 +611,16 @@
         <v>18</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="28.5">
+    <row r="8" spans="1:10" ht="45">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -695,9 +688,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -709,9 +700,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -723,9 +712,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -737,9 +724,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -752,9 +737,7 @@
     <row r="17" spans="1:10">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="1">
-        <v>9917329</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -765,16 +748,9 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5605867</v>
-      </c>
-      <c r="D18" s="1">
-        <f>C18/C17</f>
-        <v>0.56525975895324232</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -784,16 +760,9 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3160471</v>
-      </c>
-      <c r="D19" s="1">
-        <f>C19/C17</f>
-        <v>0.31868167326101615</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -803,16 +772,9 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1010607</v>
-      </c>
-      <c r="D20" s="1">
-        <f>C20/C17</f>
-        <v>0.10190314347744237</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -822,16 +784,9 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1">
-        <v>140390</v>
-      </c>
-      <c r="D21" s="1">
-        <f>C21/C17</f>
-        <v>1.415602930990794E-2</v>
-      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3236,24 +3191,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>